<commit_message>
Implemented Lifting Gear Manager modules
</commit_message>
<xml_diff>
--- a/files/system/import-grommets-sample.xlsx
+++ b/files/system/import-grommets-sample.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+  <si>
+    <t xml:space="preserve">Item Description</t>
+  </si>
   <si>
     <t xml:space="preserve">Internal ID</t>
   </si>
@@ -31,15 +34,15 @@
     <t xml:space="preserve">WL</t>
   </si>
   <si>
+    <t xml:space="preserve">Dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Qty</t>
   </si>
   <si>
-    <t xml:space="preserve">BL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dia</t>
-  </si>
-  <si>
     <t xml:space="preserve">ICC</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
     <t xml:space="preserve">Inspection Authority</t>
   </si>
   <si>
+    <t xml:space="preserve">Lifts</t>
+  </si>
+  <si>
     <t xml:space="preserve">Date of discharged</t>
   </si>
   <si>
@@ -92,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">Inspection Passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grommet-373 Ts-7.5m</t>
   </si>
   <si>
     <t xml:space="preserve">G-373-75-2</t>
@@ -426,32 +435,36 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <pane xSplit="6" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="2" width="5.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="10.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="11.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="10.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="2" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="2" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="25" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="5.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="2" width="5.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="6.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="2" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="2" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="27" style="2" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -527,109 +540,119 @@
       <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AMG1" s="6"/>
-      <c r="AMH1" s="6"/>
+      <c r="Y1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="AMI1" s="6"/>
-      <c r="AMJ1" s="6"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="8" t="n">
+        <v>26</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="8" t="n">
         <v>373</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="D2" s="9" t="n">
         <v>7.5</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="E2" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2" s="9" t="n">
+        <v>1230</v>
+      </c>
+      <c r="G2" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="n">
-        <v>1230</v>
-      </c>
-      <c r="F2" s="10" t="n">
-        <v>162</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="10" t="n">
+      <c r="H2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="K2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="12" t="n">
+      <c r="L2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="12" t="n">
         <v>39476</v>
       </c>
-      <c r="M2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="12" t="n">
+      <c r="N2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="12" t="n">
         <v>39454</v>
       </c>
-      <c r="O2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="12" t="n">
+      <c r="P2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="12" t="n">
         <v>41981</v>
       </c>
-      <c r="Q2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="12" t="n">
+      <c r="R2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="12" t="n">
         <v>44891</v>
       </c>
-      <c r="S2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="13"/>
-      <c r="U2" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="V2" s="13" t="n">
+      <c r="T2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="V2" s="13"/>
+      <c r="W2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="X2" s="13" t="n">
         <v>0</v>
       </c>
-      <c r="W2" s="13" t="n">
+      <c r="Y2" s="13" t="n">
         <v>0</v>
       </c>
-      <c r="X2" s="13" t="n">
+      <c r="Z2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="Y2" s="0"/>
-      <c r="Z2" s="0"/>
       <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="C3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="C4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="C5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Rework Lifting Gear Manager
</commit_message>
<xml_diff>
--- a/files/system/import-grommets-sample.xlsx
+++ b/files/system/import-grommets-sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t xml:space="preserve">Item Description</t>
   </si>
@@ -88,7 +88,10 @@
     <t xml:space="preserve">Date of discharged</t>
   </si>
   <si>
-    <t xml:space="preserve">Remarks</t>
+    <t xml:space="preserve">Remarks Load Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remarks Visual Inspection</t>
   </si>
   <si>
     <t xml:space="preserve">Initial Test Passed</t>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">DNV ins. &amp; Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loadtest Carried out by Master &amp; DNV Inspector in Durban 26.11.2022</t>
   </si>
   <si>
     <t xml:space="preserve">Annual Visual Inspection Carried out by Master &amp; DNV Inspector in Durban 26.11.2022</t>
@@ -290,7 +296,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -312,10 +318,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,9 +437,9 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <pane xSplit="6" ySplit="0" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -461,10 +463,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="6.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="2" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="2" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="27" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="22" style="2" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="2" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="28" style="2" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -546,113 +548,118 @@
       <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AMI1" s="6"/>
+      <c r="AA1" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="7" t="n">
         <v>373</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="8" t="n">
         <v>7.5</v>
       </c>
-      <c r="E2" s="9" t="n">
+      <c r="E2" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="F2" s="9" t="n">
+      <c r="F2" s="8" t="n">
         <v>1230</v>
       </c>
-      <c r="G2" s="9" t="n">
+      <c r="G2" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="10" t="n">
+      <c r="J2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="11" t="n">
+        <v>39476</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="11" t="n">
+        <v>39454</v>
+      </c>
+      <c r="P2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="12" t="n">
-        <v>39476</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="12" t="n">
-        <v>39454</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="12" t="n">
+      <c r="Q2" s="11" t="n">
         <v>41981</v>
       </c>
-      <c r="R2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="12" t="n">
+      <c r="R2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="11" t="n">
         <v>44891</v>
       </c>
-      <c r="T2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="13" t="n">
+      <c r="T2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="V2" s="13"/>
-      <c r="W2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="X2" s="13" t="n">
+      <c r="V2" s="12"/>
+      <c r="W2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="Y2" s="13" t="n">
+      <c r="Z2" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="Z2" s="13" t="n">
+      <c r="AA2" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
       <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="C3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="C5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="C6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Add back button, update import files
</commit_message>
<xml_diff>
--- a/files/system/import-grommets-sample.xlsx
+++ b/files/system/import-grommets-sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t xml:space="preserve">Item Description</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">Remarks Visual Inspection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial Test Passed</t>
   </si>
   <si>
     <t xml:space="preserve">Last Test Passed</t>
@@ -440,12 +437,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="0" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topRight" activeCell="Z1" activeCellId="0" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -470,9 +467,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="6.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="23" style="2" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="2" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="29" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="28" style="2" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -557,16 +554,14 @@
       <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="C2" s="7" t="n">
         <v>373</v>
@@ -575,7 +570,7 @@
         <v>7.5</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="8" t="n">
         <v>20</v>
@@ -587,66 +582,63 @@
         <v>4</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="L2" s="9" t="n">
         <v>2</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N2" s="11" t="n">
         <v>39476</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P2" s="11" t="n">
         <v>39454</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R2" s="11" t="n">
         <v>41981</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T2" s="11" t="n">
         <v>44891</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V2" s="12" t="n">
         <v>10</v>
       </c>
       <c r="W2" s="12"/>
       <c r="X2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="Y2" s="13" t="s">
-        <v>39</v>
       </c>
       <c r="Z2" s="12" t="n">
         <v>0</v>
       </c>
       <c r="AA2" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="12" t="n">
         <v>1</v>
       </c>
+      <c r="AB2" s="0"/>
       <c r="AC2" s="0"/>
       <c r="AD2" s="0"/>
-      <c r="AE2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="14"/>

</xml_diff>